<commit_message>
Spell learning changed and scholar started
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Archetypes/Sage.xlsx
+++ b/CoreRulebook/Data/Archetypes/Sage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\HPRPG\CoreRulebook\Data\Archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BE0688-1E56-4BE5-8506-6E9E28EFC969}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E841D8FD-892C-49EC-97C1-DAE88F6ECD6F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27240" yWindow="1590" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>LVL</t>
   </si>
@@ -45,16 +45,34 @@
     <t>Teacher</t>
   </si>
   <si>
-    <t>Stuff0</t>
-  </si>
-  <si>
-    <t>Stuff1</t>
-  </si>
-  <si>
-    <t>Stuff2</t>
-  </si>
-  <si>
     <t>Scholar</t>
+  </si>
+  <si>
+    <t>Instructive Aura</t>
+  </si>
+  <si>
+    <t>Guiding Hand</t>
+  </si>
+  <si>
+    <t>Guiding Hand II</t>
+  </si>
+  <si>
+    <t>Intellectual Insight</t>
+  </si>
+  <si>
+    <t>Arcane Affinity</t>
+  </si>
+  <si>
+    <t>Repository of Knowledge</t>
+  </si>
+  <si>
+    <t>Rapid Assimilation</t>
+  </si>
+  <si>
+    <t>Innovative Mind</t>
+  </si>
+  <si>
+    <t>Research Training</t>
   </si>
 </sst>
 </file>
@@ -409,14 +427,16 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="11.5703125"/>
-    <col min="3" max="4" width="41.28515625" customWidth="1"/>
-    <col min="5" max="1025" width="11.5703125"/>
+    <col min="3" max="3" width="41.28515625" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -433,7 +453,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -445,13 +465,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -459,8 +473,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -468,8 +484,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -477,8 +498,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -486,8 +509,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -495,8 +520,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -504,8 +531,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -513,8 +542,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -522,8 +550,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -531,8 +558,10 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -540,8 +569,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -549,8 +577,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -558,8 +585,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -567,8 +593,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -576,8 +601,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -585,8 +609,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -595,8 +618,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -604,8 +626,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -613,8 +634,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -622,8 +642,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>